<commit_message>
added 3d plot of average values
</commit_message>
<xml_diff>
--- a/average_values.xlsx
+++ b/average_values.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="average_values_per_location" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1056,6 +1057,1314 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:surface3DChart>
+        <c:wireframe val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>713.1955612</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.8669586222235903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>23.46148684</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>13.6701853082133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>318.2309842</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="2">
+                  <c:v>9.9945428347492395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>288.8418497</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="3">
+                  <c:v>13.2393378722679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>596.9276712</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="4">
+                  <c:v>10.1715708786938</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>25.08330438</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="5">
+                  <c:v>12.7087254671889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>976.5530945</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="6">
+                  <c:v>6.4345994238790398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>854.0491009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="7">
+                  <c:v>7.06598585039713</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>986.8277251</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="8">
+                  <c:v>5.6012837981024504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>367.6748296</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln/>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>205.85085879187099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>773.50627482098503</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.2011082066916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>422.240488752776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>565.41533443122603</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.71409053883599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482.70911384085798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834.36184485211095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.584073511676202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>788.75525642934201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="9">
+                  <c:v>12.0532224492616</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-3D7A-4C1B-B800-5FD5311AB769}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:bandFmts>
+          <c:bandFmt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="12"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="13"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+          <c:bandFmt>
+            <c:idx val="14"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln/>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+          </c:bandFmt>
+        </c:bandFmts>
+        <c:axId val="445379824"/>
+        <c:axId val="445384400"/>
+        <c:axId val="440343200"/>
+      </c:surface3DChart>
+      <c:catAx>
+        <c:axId val="445379824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445384400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="445384400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445379824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="440343200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445384400"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1647,6 +2956,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>568325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1912,8 +3256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2051,4 +3395,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>205.85085879187099</v>
+      </c>
+      <c r="C1">
+        <v>773.50627482098503</v>
+      </c>
+      <c r="D1">
+        <v>67.2011082066916</v>
+      </c>
+      <c r="E1">
+        <v>422.240488752776</v>
+      </c>
+      <c r="F1">
+        <v>565.41533443122603</v>
+      </c>
+      <c r="G1">
+        <v>239.71409053883599</v>
+      </c>
+      <c r="H1">
+        <v>482.70911384085798</v>
+      </c>
+      <c r="I1">
+        <v>834.36184485211095</v>
+      </c>
+      <c r="J1">
+        <v>33.584073511676202</v>
+      </c>
+      <c r="K1">
+        <v>788.75525642934201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>713.19556123458005</v>
+      </c>
+      <c r="B2">
+        <v>7.8669586222235903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>23.461486835845399</v>
+      </c>
+      <c r="C3">
+        <v>13.6701853082133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>318.23098423050601</v>
+      </c>
+      <c r="D4">
+        <v>9.9945428347492395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>288.84184967991598</v>
+      </c>
+      <c r="E5">
+        <v>13.2393378722679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>596.92767118336701</v>
+      </c>
+      <c r="F6">
+        <v>10.1715708786938</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>25.0833043762991</v>
+      </c>
+      <c r="G7">
+        <v>12.7087254671889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>976.55309453866096</v>
+      </c>
+      <c r="H8">
+        <v>6.4345994238790398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>854.04910093280103</v>
+      </c>
+      <c r="I9">
+        <v>7.06598585039713</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>986.82772514071303</v>
+      </c>
+      <c r="J10">
+        <v>5.6012837981024504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>367.67482955777399</v>
+      </c>
+      <c r="K11">
+        <v>12.0532224492616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>